<commit_message>
Bugfix divers >> 5.5
</commit_message>
<xml_diff>
--- a/tables/Grille-présentation du projet-S-SI.xlsx
+++ b/tables/Grille-présentation du projet-S-SI.xlsx
@@ -13,6 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Identification!$A$3:$B$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Présentation du projet'!$A$1:$O$29</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
@@ -1234,132 +1235,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1408,6 +1283,132 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1591,12 +1592,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="60745216"/>
-        <c:axId val="60833792"/>
+        <c:axId val="121891456"/>
+        <c:axId val="121975168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="60745216"/>
+        <c:axId val="121891456"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1613,14 +1613,14 @@
           </c:spPr>
         </c:majorGridlines>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="60833792"/>
+        <c:crossAx val="121975168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60833792"/>
+        <c:axId val="121975168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1630,10 +1630,10 @@
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="60745216"/>
+        <c:crossAx val="121891456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33330000000000343"/>
+        <c:majorUnit val="0.33330000000000354"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1675,7 +1675,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.75000000000000366" r="0.75000000000000366" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
+    <c:pageMargins b="0.98425196899999956" l="0.75000000000000377" r="0.75000000000000377" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1732,12 +1732,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="61008512"/>
-        <c:axId val="61211776"/>
+        <c:axId val="122163968"/>
+        <c:axId val="122165888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61008512"/>
+        <c:axId val="122163968"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1754,14 +1753,14 @@
           </c:spPr>
         </c:majorGridlines>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="61211776"/>
+        <c:crossAx val="122165888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61211776"/>
+        <c:axId val="122165888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1771,10 +1770,10 @@
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="61008512"/>
+        <c:crossAx val="122163968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33330000000000343"/>
+        <c:majorUnit val="0.33330000000000354"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1816,7 +1815,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.75000000000000366" r="0.75000000000000366" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
+    <c:pageMargins b="0.98425196899999956" l="0.75000000000000377" r="0.75000000000000377" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1873,12 +1872,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="82093184"/>
-        <c:axId val="82268544"/>
+        <c:axId val="122198656"/>
+        <c:axId val="121840000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82093184"/>
+        <c:axId val="122198656"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1895,14 +1893,14 @@
           </c:spPr>
         </c:majorGridlines>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="82268544"/>
+        <c:crossAx val="121840000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82268544"/>
+        <c:axId val="121840000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1912,10 +1910,10 @@
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="82093184"/>
+        <c:crossAx val="122198656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33330000000000343"/>
+        <c:majorUnit val="0.33330000000000354"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1957,7 +1955,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.75000000000000366" r="0.75000000000000366" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
+    <c:pageMargins b="0.98425196899999956" l="0.75000000000000377" r="0.75000000000000377" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2014,12 +2012,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="84858368"/>
-        <c:axId val="84859904"/>
+        <c:axId val="121879936"/>
+        <c:axId val="121967744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84858368"/>
+        <c:axId val="121879936"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2036,14 +2033,14 @@
           </c:spPr>
         </c:majorGridlines>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="84859904"/>
+        <c:crossAx val="121967744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84859904"/>
+        <c:axId val="121967744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2053,10 +2050,10 @@
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="84858368"/>
+        <c:crossAx val="121879936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33330000000000343"/>
+        <c:majorUnit val="0.33330000000000354"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2098,7 +2095,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.75000000000000366" r="0.75000000000000366" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
+    <c:pageMargins b="0.98425196899999956" l="0.75000000000000377" r="0.75000000000000377" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2170,12 +2167,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="109013632"/>
-        <c:axId val="115093504"/>
+        <c:axId val="121999744"/>
+        <c:axId val="122001280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109013632"/>
+        <c:axId val="121999744"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2192,14 +2188,14 @@
           </c:spPr>
         </c:majorGridlines>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="115093504"/>
+        <c:crossAx val="122001280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115093504"/>
+        <c:axId val="122001280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2209,10 +2205,10 @@
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="109013632"/>
+        <c:crossAx val="121999744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33330000000000343"/>
+        <c:majorUnit val="0.33330000000000354"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2254,7 +2250,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.75000000000000366" r="0.75000000000000366" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
+    <c:pageMargins b="0.98425196899999956" l="0.75000000000000377" r="0.75000000000000377" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2271,7 +2267,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.3691275167785095E-2"/>
-          <c:y val="2.2831152036744219E-2"/>
+          <c:y val="2.2831152036744226E-2"/>
           <c:w val="0.91946308724832049"/>
           <c:h val="0.95890838554324298"/>
         </c:manualLayout>
@@ -2354,12 +2350,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="58046336"/>
-        <c:axId val="58047872"/>
+        <c:axId val="122168448"/>
+        <c:axId val="122169984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58046336"/>
+        <c:axId val="122168448"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2376,14 +2371,14 @@
           </c:spPr>
         </c:majorGridlines>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="58047872"/>
+        <c:crossAx val="122169984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58047872"/>
+        <c:axId val="122169984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2393,10 +2388,10 @@
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="58046336"/>
+        <c:crossAx val="122168448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33330000000000343"/>
+        <c:majorUnit val="0.33330000000000354"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2438,7 +2433,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.75000000000000366" r="0.75000000000000366" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
+    <c:pageMargins b="0.98425196899999956" l="0.75000000000000377" r="0.75000000000000377" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2524,28 +2519,27 @@
             </c:numLit>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="58065664"/>
-        <c:axId val="58067200"/>
+        <c:axId val="128815104"/>
+        <c:axId val="128816640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58065664"/>
+        <c:axId val="128815104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="58067200"/>
+        <c:crossAx val="128816640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58067200"/>
+        <c:axId val="128816640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2553,7 +2547,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="58065664"/>
+        <c:crossAx val="128815104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2592,7 +2586,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.75000000000000366" r="0.75000000000000366" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
+    <c:pageMargins b="0.98425196899999956" l="0.75000000000000377" r="0.75000000000000377" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2678,28 +2672,27 @@
             </c:numLit>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="58084736"/>
-        <c:axId val="58086528"/>
+        <c:axId val="128875136"/>
+        <c:axId val="128881024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58084736"/>
+        <c:axId val="128875136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="58086528"/>
+        <c:crossAx val="128881024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58086528"/>
+        <c:axId val="128881024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2707,7 +2700,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="58084736"/>
+        <c:crossAx val="128875136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2746,7 +2739,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.75000000000000366" r="0.75000000000000366" t="0.98425196899999956" header="0.49212598450000183" footer="0.49212598450000183"/>
+    <c:pageMargins b="0.98425196899999956" l="0.75000000000000377" r="0.75000000000000377" t="0.98425196899999956" header="0.49212598450000189" footer="0.49212598450000189"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3268,7 +3261,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3534,10 +3527,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="70" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:I21"/>
+    <sheetView zoomScale="70" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3560,17 +3556,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="9" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="150" t="s">
+      <c r="B1" s="143"/>
+      <c r="C1" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
@@ -3592,14 +3588,14 @@
     <row r="2" spans="1:24" s="9" customFormat="1" ht="25.5" customHeight="1">
       <c r="A2" s="7"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
       <c r="O2" s="16"/>
@@ -3614,17 +3610,17 @@
       <c r="X2" s="67"/>
     </row>
     <row r="3" spans="1:24" s="9" customFormat="1" ht="25.5">
-      <c r="A3" s="157" t="s">
+      <c r="A3" s="144" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="158"/>
-      <c r="C3" s="152" t="s">
+      <c r="B3" s="145"/>
+      <c r="C3" s="134" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="153"/>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="154"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="136"/>
       <c r="H3" s="12">
         <v>0</v>
       </c>
@@ -3656,20 +3652,20 @@
       <c r="X3" s="67"/>
     </row>
     <row r="4" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="124" t="s">
+      <c r="A4" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
-      <c r="G4" s="125"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="126"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
+      <c r="F4" s="140"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="140"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="141"/>
       <c r="M4" s="51"/>
       <c r="N4" s="49">
         <v>0.3</v>
@@ -3695,19 +3691,19 @@
       <c r="X4" s="67"/>
     </row>
     <row r="5" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A5" s="127" t="s">
+      <c r="A5" s="165" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="129" t="s">
+      <c r="C5" s="167" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="131"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="168"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="169"/>
       <c r="H5" s="55"/>
       <c r="I5" s="55"/>
       <c r="J5" s="55"/>
@@ -3741,17 +3737,17 @@
       <c r="X5" s="67"/>
     </row>
     <row r="6" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A6" s="128"/>
+      <c r="A6" s="166"/>
       <c r="B6" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="117" t="s">
+      <c r="C6" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="119"/>
+      <c r="D6" s="159"/>
+      <c r="E6" s="159"/>
+      <c r="F6" s="159"/>
+      <c r="G6" s="160"/>
       <c r="H6" s="54"/>
       <c r="I6" s="54"/>
       <c r="J6" s="54"/>
@@ -3785,19 +3781,19 @@
       <c r="X6" s="67"/>
     </row>
     <row r="7" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A7" s="127" t="s">
+      <c r="A7" s="165" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="170" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="133"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="133"/>
-      <c r="G7" s="134"/>
+      <c r="D7" s="171"/>
+      <c r="E7" s="171"/>
+      <c r="F7" s="171"/>
+      <c r="G7" s="172"/>
       <c r="H7" s="55"/>
       <c r="I7" s="55"/>
       <c r="J7" s="55"/>
@@ -3831,17 +3827,17 @@
       <c r="X7" s="67"/>
     </row>
     <row r="8" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A8" s="135"/>
+      <c r="A8" s="173"/>
       <c r="B8" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="121" t="s">
+      <c r="C8" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="123"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="164"/>
       <c r="H8" s="56"/>
       <c r="I8" s="56"/>
       <c r="J8" s="56"/>
@@ -3875,17 +3871,17 @@
       <c r="X8" s="67"/>
     </row>
     <row r="9" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
-      <c r="A9" s="128"/>
+      <c r="A9" s="166"/>
       <c r="B9" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="132" t="s">
+      <c r="C9" s="170" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="134"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="172"/>
       <c r="H9" s="60"/>
       <c r="I9" s="60"/>
       <c r="J9" s="60"/>
@@ -3919,20 +3915,20 @@
       <c r="X9" s="67"/>
     </row>
     <row r="10" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="124" t="s">
+      <c r="A10" s="139" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="125"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="125"/>
-      <c r="G10" s="125"/>
-      <c r="H10" s="125"/>
-      <c r="I10" s="125"/>
-      <c r="J10" s="125"/>
-      <c r="K10" s="125"/>
-      <c r="L10" s="126"/>
+      <c r="B10" s="140"/>
+      <c r="C10" s="140"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="140"/>
+      <c r="G10" s="140"/>
+      <c r="H10" s="140"/>
+      <c r="I10" s="140"/>
+      <c r="J10" s="140"/>
+      <c r="K10" s="140"/>
+      <c r="L10" s="141"/>
       <c r="M10" s="51"/>
       <c r="N10" s="49">
         <v>0.3</v>
@@ -3952,19 +3948,19 @@
       <c r="X10" s="67"/>
     </row>
     <row r="11" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A11" s="136" t="s">
+      <c r="A11" s="174" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="161" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
+      <c r="D11" s="161"/>
+      <c r="E11" s="161"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="161"/>
       <c r="H11" s="56"/>
       <c r="I11" s="56"/>
       <c r="J11" s="56"/>
@@ -3998,17 +3994,17 @@
       <c r="X11" s="67"/>
     </row>
     <row r="12" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A12" s="137"/>
+      <c r="A12" s="175"/>
       <c r="B12" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="140" t="s">
+      <c r="C12" s="148" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="140"/>
-      <c r="E12" s="140"/>
-      <c r="F12" s="140"/>
-      <c r="G12" s="140"/>
+      <c r="D12" s="148"/>
+      <c r="E12" s="148"/>
+      <c r="F12" s="148"/>
+      <c r="G12" s="148"/>
       <c r="H12" s="60"/>
       <c r="I12" s="60"/>
       <c r="J12" s="60"/>
@@ -4048,13 +4044,13 @@
       <c r="B13" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="120" t="s">
+      <c r="C13" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
+      <c r="D13" s="161"/>
+      <c r="E13" s="161"/>
+      <c r="F13" s="161"/>
+      <c r="G13" s="161"/>
       <c r="H13" s="56"/>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
@@ -4088,20 +4084,20 @@
       <c r="X13" s="67"/>
     </row>
     <row r="14" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="152" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="145"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="145"/>
-      <c r="E14" s="145"/>
-      <c r="F14" s="145"/>
-      <c r="G14" s="145"/>
-      <c r="H14" s="145"/>
-      <c r="I14" s="145"/>
-      <c r="J14" s="145"/>
-      <c r="K14" s="145"/>
-      <c r="L14" s="145"/>
+      <c r="B14" s="153"/>
+      <c r="C14" s="153"/>
+      <c r="D14" s="153"/>
+      <c r="E14" s="153"/>
+      <c r="F14" s="153"/>
+      <c r="G14" s="153"/>
+      <c r="H14" s="153"/>
+      <c r="I14" s="153"/>
+      <c r="J14" s="153"/>
+      <c r="K14" s="153"/>
+      <c r="L14" s="153"/>
       <c r="M14" s="53"/>
       <c r="N14" s="49">
         <v>0.4</v>
@@ -4127,13 +4123,13 @@
       <c r="B15" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="141" t="s">
+      <c r="C15" s="149" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="142"/>
-      <c r="E15" s="142"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="143"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="150"/>
+      <c r="F15" s="150"/>
+      <c r="G15" s="151"/>
       <c r="H15" s="75"/>
       <c r="I15" s="75"/>
       <c r="J15" s="75"/>
@@ -4167,19 +4163,19 @@
       <c r="X15" s="67"/>
     </row>
     <row r="16" spans="1:24" ht="27.75" customHeight="1">
-      <c r="A16" s="146" t="s">
+      <c r="A16" s="154" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="147" t="s">
+      <c r="C16" s="155" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="147"/>
-      <c r="E16" s="147"/>
-      <c r="F16" s="147"/>
-      <c r="G16" s="147"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
       <c r="H16" s="63"/>
       <c r="I16" s="63"/>
       <c r="J16" s="63"/>
@@ -4213,17 +4209,17 @@
       <c r="X16" s="70"/>
     </row>
     <row r="17" spans="1:24" ht="27.75" customHeight="1">
-      <c r="A17" s="146"/>
+      <c r="A17" s="154"/>
       <c r="B17" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="140" t="s">
+      <c r="C17" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="140"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
+      <c r="D17" s="148"/>
+      <c r="E17" s="148"/>
+      <c r="F17" s="148"/>
+      <c r="G17" s="148"/>
       <c r="H17" s="75"/>
       <c r="I17" s="75"/>
       <c r="J17" s="75"/>
@@ -4257,17 +4253,17 @@
       <c r="X17" s="70"/>
     </row>
     <row r="18" spans="1:24" ht="30.75" customHeight="1">
-      <c r="A18" s="146"/>
+      <c r="A18" s="154"/>
       <c r="B18" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="148" t="s">
+      <c r="C18" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="148"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="148"/>
-      <c r="G18" s="148"/>
+      <c r="D18" s="156"/>
+      <c r="E18" s="156"/>
+      <c r="F18" s="156"/>
+      <c r="G18" s="156"/>
       <c r="H18" s="63"/>
       <c r="I18" s="63"/>
       <c r="J18" s="63"/>
@@ -4328,22 +4324,22 @@
     </row>
     <row r="20" spans="1:24" ht="27.75" customHeight="1">
       <c r="B20" s="9"/>
-      <c r="C20" s="149" t="s">
+      <c r="C20" s="157" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="149"/>
-      <c r="E20" s="149"/>
-      <c r="F20" s="149"/>
-      <c r="G20" s="149"/>
-      <c r="H20" s="139" t="str">
+      <c r="D20" s="157"/>
+      <c r="E20" s="157"/>
+      <c r="F20" s="157"/>
+      <c r="G20" s="157"/>
+      <c r="H20" s="147" t="str">
         <f>IF(S4=0,"!",O4+O10+O14)</f>
         <v>!</v>
       </c>
-      <c r="I20" s="139"/>
-      <c r="J20" s="138" t="s">
+      <c r="I20" s="147"/>
+      <c r="J20" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="K20" s="138"/>
+      <c r="K20" s="146"/>
       <c r="O20" s="16"/>
       <c r="P20" s="69"/>
       <c r="Q20" s="105"/>
@@ -4357,19 +4353,19 @@
     </row>
     <row r="21" spans="1:24" ht="26.25" customHeight="1">
       <c r="B21" s="9"/>
-      <c r="C21" s="163" t="s">
+      <c r="C21" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="164"/>
-      <c r="E21" s="164"/>
-      <c r="F21" s="164"/>
-      <c r="G21" s="165"/>
-      <c r="H21" s="166"/>
-      <c r="I21" s="166"/>
-      <c r="J21" s="171" t="s">
+      <c r="D21" s="122"/>
+      <c r="E21" s="122"/>
+      <c r="F21" s="122"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="124"/>
+      <c r="J21" s="129" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="172"/>
+      <c r="K21" s="130"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="O21" s="16"/>
@@ -4407,12 +4403,12 @@
       <c r="B23" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="162" t="s">
+      <c r="C23" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="162"/>
-      <c r="E23" s="162"/>
-      <c r="F23" s="162"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="120"/>
       <c r="H23" s="78"/>
       <c r="I23" s="78"/>
       <c r="J23" s="78"/>
@@ -4431,17 +4427,17 @@
       <c r="X23" s="70"/>
     </row>
     <row r="24" spans="1:24" ht="12.75" customHeight="1">
-      <c r="B24" s="167" t="str">
+      <c r="B24" s="125" t="str">
         <f>CONCATENATE(Identification!B9," ",Identification!B10)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C24" s="167" t="str">
+      <c r="C24" s="125" t="str">
         <f>CONCATENATE(Identification!B7," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D24" s="167"/>
-      <c r="E24" s="167"/>
-      <c r="F24" s="167"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="125"/>
+      <c r="F24" s="125"/>
       <c r="H24" s="78"/>
       <c r="I24" s="78"/>
       <c r="J24" s="78"/>
@@ -4460,11 +4456,11 @@
       <c r="X24" s="70"/>
     </row>
     <row r="25" spans="1:24" ht="13.5" customHeight="1">
-      <c r="B25" s="167"/>
-      <c r="C25" s="167"/>
-      <c r="D25" s="167"/>
-      <c r="E25" s="167"/>
-      <c r="F25" s="167"/>
+      <c r="B25" s="125"/>
+      <c r="C25" s="125"/>
+      <c r="D25" s="125"/>
+      <c r="E25" s="125"/>
+      <c r="F25" s="125"/>
       <c r="H25" s="72"/>
       <c r="I25" s="70"/>
       <c r="J25" s="70"/>
@@ -4483,11 +4479,11 @@
       <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:24" ht="14.25" thickBot="1">
-      <c r="B26" s="167"/>
-      <c r="C26" s="167"/>
-      <c r="D26" s="167"/>
-      <c r="E26" s="167"/>
-      <c r="F26" s="167"/>
+      <c r="B26" s="125"/>
+      <c r="C26" s="125"/>
+      <c r="D26" s="125"/>
+      <c r="E26" s="125"/>
+      <c r="F26" s="125"/>
       <c r="H26" s="40"/>
       <c r="I26" s="80"/>
       <c r="J26" s="40"/>
@@ -4509,18 +4505,18 @@
       <c r="B27" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="152" t="s">
+      <c r="C27" s="134" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="153"/>
-      <c r="E27" s="153"/>
-      <c r="F27" s="154"/>
-      <c r="H27" s="173" t="s">
+      <c r="D27" s="135"/>
+      <c r="E27" s="135"/>
+      <c r="F27" s="136"/>
+      <c r="H27" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="I27" s="174"/>
-      <c r="J27" s="174"/>
-      <c r="K27" s="175"/>
+      <c r="I27" s="132"/>
+      <c r="J27" s="132"/>
+      <c r="K27" s="133"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="O27" s="16"/>
@@ -4539,17 +4535,17 @@
         <f>CONCATENATE(Identification!B18," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C28" s="159" t="str">
+      <c r="C28" s="117" t="str">
         <f>CONCATENATE(Identification!C18," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D28" s="160"/>
-      <c r="E28" s="160"/>
-      <c r="F28" s="161"/>
-      <c r="H28" s="168"/>
-      <c r="I28" s="169"/>
-      <c r="J28" s="169"/>
-      <c r="K28" s="170"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="119"/>
+      <c r="H28" s="126"/>
+      <c r="I28" s="127"/>
+      <c r="J28" s="127"/>
+      <c r="K28" s="128"/>
       <c r="L28" s="42"/>
       <c r="M28" s="42"/>
       <c r="O28" s="16"/>
@@ -4568,13 +4564,13 @@
         <f>CONCATENATE(Identification!B19," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C29" s="159" t="str">
+      <c r="C29" s="117" t="str">
         <f>CONCATENATE(Identification!C19," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D29" s="160"/>
-      <c r="E29" s="160"/>
-      <c r="F29" s="161"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="119"/>
       <c r="O29" s="16"/>
       <c r="P29" s="69"/>
       <c r="Q29" s="70"/>
@@ -4743,6 +4739,34 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" pivotTables="0"/>
   <mergeCells count="39">
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="H2:K2"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="C21:G21"/>
@@ -4754,34 +4778,6 @@
     <mergeCell ref="H27:K27"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="H21:I21">
@@ -4817,8 +4813,8 @@
       <formula>$L$28</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.37" right="0.31" top="0.43" bottom="0.36" header="0.51181102362204722" footer="0.36"/>
+  <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Bugfix : enregistrement grilles dans fichier original
</commit_message>
<xml_diff>
--- a/tables/Grille-présentation du projet-S-SI.xlsx
+++ b/tables/Grille-présentation du projet-S-SI.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cedrick\Documents\Developp\pysequence\tables\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="345" windowWidth="11130" windowHeight="6255"/>
+    <workbookView xWindow="660" yWindow="350" windowWidth="11130" windowHeight="6260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Notice à lire" sheetId="5" r:id="rId1"/>
@@ -12,10 +17,10 @@
     <sheet name="Présentation du projet" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Identification!$A$3:$B$14</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Présentation du projet'!$A$1:$O$29</definedName>
+    <definedName name="Print_Area" localSheetId="1">Identification!$A$3:$B$14</definedName>
+    <definedName name="Print_Area" localSheetId="2">'Présentation du projet'!$A$1:$O$29</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -270,11 +275,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1537,19 +1542,34 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1590,8 +1610,20 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8753-41B9-AC34-AFA445DBEF6C}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="121891456"/>
         <c:axId val="121975168"/>
       </c:barChart>
@@ -1612,12 +1644,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="121975168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="121975168"/>
@@ -1629,6 +1664,8 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="121891456"/>
         <c:crosses val="autoZero"/>
@@ -1649,6 +1686,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -1682,14 +1720,26 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1730,8 +1780,20 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5972-4493-A288-3CF85CD0886A}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="122163968"/>
         <c:axId val="122165888"/>
       </c:barChart>
@@ -1752,12 +1814,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="122165888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="122165888"/>
@@ -1769,6 +1834,8 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="122163968"/>
         <c:crosses val="autoZero"/>
@@ -1789,6 +1856,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -1822,14 +1890,26 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1870,8 +1950,20 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C35-4214-8A5B-E3176F2F896A}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="122198656"/>
         <c:axId val="121840000"/>
       </c:barChart>
@@ -1892,12 +1984,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="121840000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="121840000"/>
@@ -1909,6 +2004,8 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="122198656"/>
         <c:crosses val="autoZero"/>
@@ -1929,6 +2026,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -1962,14 +2060,26 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2010,8 +2120,20 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5FA8-49C3-BF86-15D42FE733DF}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="121879936"/>
         <c:axId val="121967744"/>
       </c:barChart>
@@ -2032,12 +2154,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="121967744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="121967744"/>
@@ -2049,6 +2174,8 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="121879936"/>
         <c:crosses val="autoZero"/>
@@ -2069,6 +2196,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -2102,14 +2230,26 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2165,8 +2305,20 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-21E8-4B2E-BC42-7A6471EB28DD}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="121999744"/>
         <c:axId val="122001280"/>
       </c:barChart>
@@ -2187,12 +2339,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="122001280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="122001280"/>
@@ -2204,6 +2359,8 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="121999744"/>
         <c:crosses val="autoZero"/>
@@ -2224,6 +2381,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -2257,9 +2415,20 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2275,6 +2444,7 @@
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2348,8 +2518,20 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1933-4DEF-8AFB-7D582D4E5204}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="122168448"/>
         <c:axId val="122169984"/>
       </c:barChart>
@@ -2370,12 +2552,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="122169984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="122169984"/>
@@ -2387,6 +2572,8 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="122168448"/>
         <c:crosses val="autoZero"/>
@@ -2407,6 +2594,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -2440,14 +2628,26 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2462,8 +2662,11 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000"/>
@@ -2475,6 +2678,11 @@
                 <a:prstDash val="solid"/>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-875E-46BF-8D62-B567F1B0A21F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numLit>
@@ -2485,6 +2693,11 @@
               </c:pt>
             </c:numLit>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-875E-46BF-8D62-B567F1B0A21F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2500,14 +2713,22 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="25400">
                 <a:noFill/>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-875E-46BF-8D62-B567F1B0A21F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numLit>
@@ -2518,7 +2739,20 @@
               </c:pt>
             </c:numLit>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-875E-46BF-8D62-B567F1B0A21F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
         <c:axId val="128815104"/>
@@ -2531,12 +2765,15 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="128816640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="128816640"/>
@@ -2546,6 +2783,8 @@
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="128815104"/>
         <c:crosses val="autoZero"/>
@@ -2560,6 +2799,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -2593,14 +2833,26 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2615,8 +2867,11 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="000000"/>
@@ -2628,6 +2883,11 @@
                 <a:prstDash val="solid"/>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-3E18-4817-929E-1B6A998C7001}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numLit>
@@ -2638,6 +2898,11 @@
               </c:pt>
             </c:numLit>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3E18-4817-929E-1B6A998C7001}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2653,14 +2918,22 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln w="25400">
                 <a:noFill/>
               </a:ln>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-3E18-4817-929E-1B6A998C7001}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numLit>
@@ -2671,7 +2944,20 @@
               </c:pt>
             </c:numLit>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3E18-4817-929E-1B6A998C7001}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
         <c:axId val="128875136"/>
@@ -2684,12 +2970,15 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="128881024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="128881024"/>
@@ -2699,6 +2988,8 @@
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="128875136"/>
         <c:crosses val="autoZero"/>
@@ -2713,6 +3004,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -2747,6 +3039,66 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>292100</xdr:colOff>
+          <xdr:row>63</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2050" name="Objet 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -2762,7 +3114,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3073" name="Graphique 1"/>
+        <xdr:cNvPr id="3073" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000010C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2794,7 +3152,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3074" name="Graphique 2"/>
+        <xdr:cNvPr id="3074" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000020C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2826,7 +3190,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3075" name="Graphique 6"/>
+        <xdr:cNvPr id="3075" name="Graphique 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000030C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2858,7 +3228,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3076" name="Graphique 8"/>
+        <xdr:cNvPr id="3076" name="Graphique 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000040C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2890,7 +3266,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3077" name="Graphique 16"/>
+        <xdr:cNvPr id="3077" name="Graphique 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000050C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2922,7 +3304,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3078" name="Graphique 21"/>
+        <xdr:cNvPr id="3078" name="Graphique 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000060C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2954,7 +3342,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3079" name="Graphique 29"/>
+        <xdr:cNvPr id="3079" name="Graphique 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000070C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2986,7 +3380,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3080" name="Graphique 33"/>
+        <xdr:cNvPr id="3080" name="Graphique 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000080C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3261,67 +3661,92 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <oleObjects>
-    <oleObject progId="Word.Document.8" shapeId="2050" r:id="rId3"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Word.Document.8" shapeId="2050" r:id="rId4">
+          <objectPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>419100</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>14</xdr:col>
+                <xdr:colOff>292100</xdr:colOff>
+                <xdr:row>63</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Word.Document.8" shapeId="2050" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="104.85546875" style="23" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="104.81640625" style="23" customWidth="1"/>
     <col min="3" max="3" width="41" style="23" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="23"/>
+    <col min="4" max="16384" width="10.81640625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A1" s="113" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="113"/>
     </row>
-    <row r="2" spans="1:3" ht="13.5" thickBot="1"/>
-    <row r="3" spans="1:3" ht="13.5" thickTop="1">
+    <row r="2" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" ht="13.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="114" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="115"/>
     </row>
-    <row r="4" spans="1:3" ht="12.75" customHeight="1">
+    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="86" t="s">
         <v>52</v>
       </c>
@@ -3329,7 +3754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
         <v>53</v>
       </c>
@@ -3337,7 +3762,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="85" t="s">
         <v>54</v>
       </c>
@@ -3345,64 +3770,64 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="25.5">
+    <row r="7" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="85" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="85" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="85" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="13.5" thickBot="1">
+    <row r="11" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="111"/>
       <c r="B11" s="112"/>
     </row>
-    <row r="12" spans="1:3" ht="13.5" thickBot="1">
+    <row r="12" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="92" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="93"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="108" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="108"/>
       <c r="C13" s="84"/>
     </row>
-    <row r="14" spans="1:3" ht="87.75" customHeight="1" thickBot="1">
+    <row r="14" spans="1:3" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="109"/>
       <c r="B14" s="110"/>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
     </row>
-    <row r="16" spans="1:3" ht="12.75" customHeight="1" thickBot="1">
+    <row r="16" spans="1:3" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="116" t="s">
         <v>61</v>
       </c>
       <c r="B16" s="116"/>
       <c r="C16" s="116"/>
     </row>
-    <row r="17" spans="1:13" ht="12.75" customHeight="1">
+    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
       <c r="B17" s="30" t="s">
         <v>41</v>
@@ -3411,23 +3836,23 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16.5" customHeight="1">
+    <row r="18" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="107" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="94"/>
       <c r="C18" s="94"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" customHeight="1">
+    <row r="19" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="107"/>
       <c r="B19" s="94"/>
       <c r="C19" s="94"/>
     </row>
-    <row r="20" spans="1:13" ht="11.25" customHeight="1">
+    <row r="20" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="25"/>
     </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1">
+    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="81"/>
       <c r="C21" s="77"/>
       <c r="D21" s="77"/>
@@ -3441,7 +3866,7 @@
       <c r="L21" s="77"/>
       <c r="M21" s="77"/>
     </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1">
+    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="81"/>
       <c r="C22" s="77"/>
       <c r="D22" s="77"/>
@@ -3455,7 +3880,7 @@
       <c r="L22" s="77"/>
       <c r="M22" s="77"/>
     </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1">
+    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="81"/>
       <c r="C23" s="77"/>
       <c r="D23" s="77"/>
@@ -3526,7 +3951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3536,26 +3961,26 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="7.26953125" style="37" customWidth="1"/>
     <col min="2" max="2" width="64" style="18" customWidth="1"/>
-    <col min="3" max="6" width="15.28515625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="2.28515625" style="18" customWidth="1"/>
-    <col min="8" max="11" width="5.140625" style="7" customWidth="1"/>
+    <col min="3" max="6" width="15.26953125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="2.26953125" style="18" customWidth="1"/>
+    <col min="8" max="11" width="5.1796875" style="7" customWidth="1"/>
     <col min="12" max="12" width="3" style="8" customWidth="1"/>
-    <col min="13" max="13" width="4.28515625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" style="15" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="44" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" style="17" customWidth="1"/>
-    <col min="17" max="17" width="5.140625" style="18" customWidth="1"/>
-    <col min="18" max="18" width="5.28515625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="4.26953125" style="8" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" style="15" customWidth="1"/>
+    <col min="15" max="15" width="10.7265625" style="44" customWidth="1"/>
+    <col min="16" max="16" width="5.81640625" style="17" customWidth="1"/>
+    <col min="17" max="17" width="5.1796875" style="18" customWidth="1"/>
+    <col min="18" max="18" width="5.26953125" style="18" customWidth="1"/>
     <col min="19" max="19" width="6" style="18" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" style="18" customWidth="1"/>
-    <col min="21" max="16384" width="11.42578125" style="18"/>
+    <col min="20" max="20" width="5.1796875" style="18" customWidth="1"/>
+    <col min="21" max="16384" width="11.453125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="9" customFormat="1" ht="30" customHeight="1">
+    <row r="1" spans="1:24" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="142" t="s">
         <v>5</v>
       </c>
@@ -3585,7 +4010,7 @@
       <c r="W1" s="67"/>
       <c r="X1" s="67"/>
     </row>
-    <row r="2" spans="1:24" s="9" customFormat="1" ht="25.5" customHeight="1">
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="C2" s="10"/>
       <c r="D2" s="138"/>
@@ -3609,7 +4034,7 @@
       <c r="W2" s="67"/>
       <c r="X2" s="67"/>
     </row>
-    <row r="3" spans="1:24" s="9" customFormat="1" ht="25.5">
+    <row r="3" spans="1:24" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.25">
       <c r="A3" s="144" t="s">
         <v>36</v>
       </c>
@@ -3651,7 +4076,7 @@
       <c r="W3" s="67"/>
       <c r="X3" s="67"/>
     </row>
-    <row r="4" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="139" t="s">
         <v>33</v>
       </c>
@@ -3690,7 +4115,7 @@
       <c r="W4" s="67"/>
       <c r="X4" s="67"/>
     </row>
-    <row r="5" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
+    <row r="5" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="165" t="s">
         <v>17</v>
       </c>
@@ -3736,7 +4161,7 @@
       <c r="W5" s="67"/>
       <c r="X5" s="67"/>
     </row>
-    <row r="6" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
+    <row r="6" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="166"/>
       <c r="B6" s="87" t="s">
         <v>12</v>
@@ -3780,7 +4205,7 @@
       <c r="W6" s="67"/>
       <c r="X6" s="67"/>
     </row>
-    <row r="7" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
+    <row r="7" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="165" t="s">
         <v>18</v>
       </c>
@@ -3826,7 +4251,7 @@
       <c r="W7" s="67"/>
       <c r="X7" s="67"/>
     </row>
-    <row r="8" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
+    <row r="8" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="173"/>
       <c r="B8" s="87" t="s">
         <v>14</v>
@@ -3870,7 +4295,7 @@
       <c r="W8" s="67"/>
       <c r="X8" s="67"/>
     </row>
-    <row r="9" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1">
+    <row r="9" spans="1:24" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="166"/>
       <c r="B9" s="87" t="s">
         <v>15</v>
@@ -3914,7 +4339,7 @@
       <c r="W9" s="67"/>
       <c r="X9" s="67"/>
     </row>
-    <row r="10" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="139" t="s">
         <v>44</v>
       </c>
@@ -3947,7 +4372,7 @@
       <c r="W10" s="67"/>
       <c r="X10" s="67"/>
     </row>
-    <row r="11" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1">
+    <row r="11" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="174" t="s">
         <v>7</v>
       </c>
@@ -3993,7 +4418,7 @@
       <c r="W11" s="67"/>
       <c r="X11" s="67"/>
     </row>
-    <row r="12" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1">
+    <row r="12" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="175"/>
       <c r="B12" s="89" t="s">
         <v>21</v>
@@ -4037,7 +4462,7 @@
       <c r="W12" s="67"/>
       <c r="X12" s="67"/>
     </row>
-    <row r="13" spans="1:24" s="9" customFormat="1" ht="28.5" customHeight="1">
+    <row r="13" spans="1:24" s="9" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>8</v>
       </c>
@@ -4083,7 +4508,7 @@
       <c r="W13" s="67"/>
       <c r="X13" s="67"/>
     </row>
-    <row r="14" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1">
+    <row r="14" spans="1:24" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="152" t="s">
         <v>60</v>
       </c>
@@ -4116,7 +4541,7 @@
       <c r="W14" s="67"/>
       <c r="X14" s="67"/>
     </row>
-    <row r="15" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1">
+    <row r="15" spans="1:24" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>9</v>
       </c>
@@ -4162,7 +4587,7 @@
       <c r="W15" s="67"/>
       <c r="X15" s="67"/>
     </row>
-    <row r="16" spans="1:24" ht="27.75" customHeight="1">
+    <row r="16" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="154" t="s">
         <v>10</v>
       </c>
@@ -4208,7 +4633,7 @@
       <c r="W16" s="70"/>
       <c r="X16" s="70"/>
     </row>
-    <row r="17" spans="1:24" ht="27.75" customHeight="1">
+    <row r="17" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="154"/>
       <c r="B17" s="91" t="s">
         <v>25</v>
@@ -4252,7 +4677,7 @@
       <c r="W17" s="70"/>
       <c r="X17" s="70"/>
     </row>
-    <row r="18" spans="1:24" ht="30.75" customHeight="1">
+    <row r="18" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="154"/>
       <c r="B18" s="91" t="s">
         <v>26</v>
@@ -4296,7 +4721,7 @@
       <c r="W18" s="70"/>
       <c r="X18" s="70"/>
     </row>
-    <row r="19" spans="1:24" ht="20.25" customHeight="1">
+    <row r="19" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="22"/>
       <c r="C19" s="34"/>
@@ -4322,7 +4747,7 @@
       <c r="W19" s="70"/>
       <c r="X19" s="70"/>
     </row>
-    <row r="20" spans="1:24" ht="27.75" customHeight="1">
+    <row r="20" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="157" t="s">
         <v>38</v>
@@ -4351,7 +4776,7 @@
       <c r="W20" s="70"/>
       <c r="X20" s="70"/>
     </row>
-    <row r="21" spans="1:24" ht="26.25" customHeight="1">
+    <row r="21" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="121" t="s">
         <v>62</v>
@@ -4379,7 +4804,7 @@
       <c r="W21" s="70"/>
       <c r="X21" s="70"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75">
+    <row r="22" spans="1:24" ht="15.5" x14ac:dyDescent="0.25">
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="H22" s="20"/>
@@ -4399,7 +4824,7 @@
       <c r="W22" s="70"/>
       <c r="X22" s="70"/>
     </row>
-    <row r="23" spans="1:24" ht="15.75">
+    <row r="23" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="82" t="s">
         <v>40</v>
       </c>
@@ -4426,7 +4851,7 @@
       <c r="W23" s="70"/>
       <c r="X23" s="70"/>
     </row>
-    <row r="24" spans="1:24" ht="12.75" customHeight="1">
+    <row r="24" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="125" t="str">
         <f>CONCATENATE(Identification!B9," ",Identification!B10)</f>
         <v xml:space="preserve"> </v>
@@ -4455,7 +4880,7 @@
       <c r="W24" s="70"/>
       <c r="X24" s="70"/>
     </row>
-    <row r="25" spans="1:24" ht="13.5" customHeight="1">
+    <row r="25" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="125"/>
       <c r="C25" s="125"/>
       <c r="D25" s="125"/>
@@ -4478,7 +4903,7 @@
       <c r="W25" s="70"/>
       <c r="X25" s="70"/>
     </row>
-    <row r="26" spans="1:24" ht="14.25" thickBot="1">
+    <row r="26" spans="1:24" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="125"/>
       <c r="C26" s="125"/>
       <c r="D26" s="125"/>
@@ -4501,7 +4926,7 @@
       <c r="W26" s="70"/>
       <c r="X26" s="70"/>
     </row>
-    <row r="27" spans="1:24" ht="25.5">
+    <row r="27" spans="1:24" ht="26" x14ac:dyDescent="0.3">
       <c r="B27" s="83" t="s">
         <v>50</v>
       </c>
@@ -4530,7 +4955,7 @@
       <c r="W27" s="70"/>
       <c r="X27" s="70"/>
     </row>
-    <row r="28" spans="1:24" ht="13.5" thickBot="1">
+    <row r="28" spans="1:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="95" t="str">
         <f>CONCATENATE(Identification!B18," ")</f>
         <v xml:space="preserve"> </v>
@@ -4559,7 +4984,7 @@
       <c r="W28" s="70"/>
       <c r="X28" s="70"/>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" ht="13" x14ac:dyDescent="0.3">
       <c r="B29" s="96" t="str">
         <f>CONCATENATE(Identification!B19," ")</f>
         <v xml:space="preserve"> </v>
@@ -4582,7 +5007,7 @@
       <c r="W29" s="70"/>
       <c r="X29" s="70"/>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O30" s="16"/>
       <c r="P30" s="69"/>
       <c r="Q30" s="70"/>
@@ -4594,7 +5019,7 @@
       <c r="W30" s="70"/>
       <c r="X30" s="70"/>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O31" s="16"/>
       <c r="P31" s="69"/>
       <c r="Q31" s="70"/>
@@ -4606,7 +5031,7 @@
       <c r="W31" s="70"/>
       <c r="X31" s="70"/>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L32" s="43"/>
       <c r="M32" s="43"/>
       <c r="O32" s="16"/>
@@ -4620,7 +5045,7 @@
       <c r="W32" s="70"/>
       <c r="X32" s="70"/>
     </row>
-    <row r="33" spans="15:24">
+    <row r="33" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O33" s="16"/>
       <c r="P33" s="69"/>
       <c r="Q33" s="70"/>
@@ -4632,7 +5057,7 @@
       <c r="W33" s="70"/>
       <c r="X33" s="70"/>
     </row>
-    <row r="34" spans="15:24">
+    <row r="34" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O34" s="16"/>
       <c r="P34" s="69"/>
       <c r="Q34" s="70"/>
@@ -4644,7 +5069,7 @@
       <c r="W34" s="70"/>
       <c r="X34" s="70"/>
     </row>
-    <row r="35" spans="15:24">
+    <row r="35" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O35" s="16"/>
       <c r="P35" s="69"/>
       <c r="Q35" s="70"/>
@@ -4656,7 +5081,7 @@
       <c r="W35" s="70"/>
       <c r="X35" s="70"/>
     </row>
-    <row r="36" spans="15:24">
+    <row r="36" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O36" s="16"/>
       <c r="P36" s="32"/>
       <c r="Q36" s="38"/>
@@ -4664,7 +5089,7 @@
       <c r="S36" s="38"/>
       <c r="T36" s="38"/>
     </row>
-    <row r="37" spans="15:24">
+    <row r="37" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O37" s="16"/>
       <c r="P37" s="32"/>
       <c r="Q37" s="38"/>
@@ -4672,7 +5097,7 @@
       <c r="S37" s="38"/>
       <c r="T37" s="38"/>
     </row>
-    <row r="38" spans="15:24">
+    <row r="38" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O38" s="16"/>
       <c r="P38" s="32"/>
       <c r="Q38" s="38"/>
@@ -4680,7 +5105,7 @@
       <c r="S38" s="38"/>
       <c r="T38" s="38"/>
     </row>
-    <row r="39" spans="15:24">
+    <row r="39" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O39" s="16"/>
       <c r="P39" s="32"/>
       <c r="Q39" s="38"/>
@@ -4688,7 +5113,7 @@
       <c r="S39" s="38"/>
       <c r="T39" s="38"/>
     </row>
-    <row r="40" spans="15:24">
+    <row r="40" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O40" s="16"/>
       <c r="P40" s="32"/>
       <c r="Q40" s="38"/>
@@ -4696,7 +5121,7 @@
       <c r="S40" s="38"/>
       <c r="T40" s="38"/>
     </row>
-    <row r="41" spans="15:24">
+    <row r="41" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O41" s="16"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="38"/>
@@ -4704,7 +5129,7 @@
       <c r="S41" s="38"/>
       <c r="T41" s="38"/>
     </row>
-    <row r="42" spans="15:24">
+    <row r="42" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O42" s="16"/>
       <c r="P42" s="32"/>
       <c r="Q42" s="38"/>
@@ -4712,7 +5137,7 @@
       <c r="S42" s="38"/>
       <c r="T42" s="38"/>
     </row>
-    <row r="43" spans="15:24">
+    <row r="43" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O43" s="16"/>
       <c r="P43" s="32"/>
       <c r="Q43" s="38"/>
@@ -4720,7 +5145,7 @@
       <c r="S43" s="38"/>
       <c r="T43" s="38"/>
     </row>
-    <row r="44" spans="15:24">
+    <row r="44" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O44" s="16"/>
       <c r="P44" s="32"/>
       <c r="Q44" s="38"/>
@@ -4728,7 +5153,7 @@
       <c r="S44" s="38"/>
       <c r="T44" s="38"/>
     </row>
-    <row r="45" spans="15:24">
+    <row r="45" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O45" s="16"/>
       <c r="P45" s="32"/>
       <c r="Q45" s="38"/>

</xml_diff>